<commit_message>
recoding some things i think are mistakes
</commit_message>
<xml_diff>
--- a/data/ideophones_coded.xlsx
+++ b/data/ideophones_coded.xlsx
@@ -3386,8 +3386,8 @@
   <dimension ref="A1:AR240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H184" sqref="H184"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16756,7 +16756,7 @@
         <v>453</v>
       </c>
       <c r="I112">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J112">
         <v>1</v>

</xml_diff>